<commit_message>
Updated data in photo report teble
</commit_message>
<xml_diff>
--- a/Marvel/Content/file/PhotoReport.xlsx
+++ b/Marvel/Content/file/PhotoReport.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phong/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979AB410-66B0-DB40-89EF-DEF41926EBB8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25460" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11145"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="38">
   <si>
     <t>Armstrong Clinic</t>
   </si>
@@ -129,15 +128,6 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>LG</t>
-  </si>
-  <si>
-    <t>HTC</t>
-  </si>
-  <si>
-    <t>Motorola</t>
-  </si>
-  <si>
     <t>Clinic F</t>
   </si>
   <si>
@@ -145,12 +135,15 @@
   </si>
   <si>
     <t>CF-0938</t>
+  </si>
+  <si>
+    <t>Tecno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -190,7 +183,7 @@
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -206,17 +199,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H23" totalsRowShown="0">
-  <autoFilter ref="A1:H23" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H23" totalsRowShown="0">
+  <autoFilter ref="A1:H23"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Photo ID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Clinic ID"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Clinic Name"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Status"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Device"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Firmware"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Flash light"/>
+    <tableColumn id="1" name="Photo ID"/>
+    <tableColumn id="2" name="Clinic ID"/>
+    <tableColumn id="3" name="Clinic Name"/>
+    <tableColumn id="4" name="Date" dataDxfId="0"/>
+    <tableColumn id="5" name="Status"/>
+    <tableColumn id="6" name="Device"/>
+    <tableColumn id="7" name="Firmware"/>
+    <tableColumn id="8" name="Flash light"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -518,23 +511,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="8" max="8" width="11.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -560,7 +553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -568,7 +561,7 @@
         <v>12873</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D2" s="2">
         <v>43556.423611111109</v>
@@ -586,7 +579,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -594,7 +587,7 @@
         <v>12873</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D3" s="2">
         <v>43556.798611111109</v>
@@ -603,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -612,7 +605,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -620,7 +613,7 @@
         <v>12873</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2">
         <v>43558.8125</v>
@@ -629,7 +622,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G4">
         <v>4</v>
@@ -638,7 +631,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -646,7 +639,7 @@
         <v>12873</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D5" s="2">
         <v>43559.423611111109</v>
@@ -655,7 +648,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -664,7 +657,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -672,7 +665,7 @@
         <v>12873</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2">
         <v>43565.756944444445</v>
@@ -690,7 +683,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -698,7 +691,7 @@
         <v>12873</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2">
         <v>43570.840277777781</v>
@@ -707,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -716,7 +709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -724,7 +717,7 @@
         <v>12873</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D8" s="2">
         <v>43575.923611111109</v>
@@ -733,7 +726,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G8">
         <v>4</v>
@@ -742,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -750,7 +743,7 @@
         <v>12873</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2">
         <v>43575.854166666664</v>
@@ -768,7 +761,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -776,7 +769,7 @@
         <v>12873</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" s="2">
         <v>43580.822916666664</v>
@@ -785,7 +778,7 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G10">
         <v>4</v>
@@ -794,7 +787,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -802,7 +795,7 @@
         <v>12873</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2">
         <v>43580.90625</v>
@@ -820,15 +813,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B12">
         <v>12873</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2">
         <v>43581.760416666664</v>
@@ -846,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -863,7 +856,7 @@
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -872,7 +865,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -889,7 +882,7 @@
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G14">
         <v>4</v>
@@ -898,7 +891,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -915,7 +908,7 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G15">
         <v>4</v>
@@ -924,7 +917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -941,7 +934,7 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -950,7 +943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -967,7 +960,7 @@
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G17">
         <v>4</v>
@@ -976,7 +969,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -993,7 +986,7 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G18">
         <v>4</v>
@@ -1002,7 +995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1019,7 +1012,7 @@
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G19">
         <v>4</v>
@@ -1028,7 +1021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1045,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G20">
         <v>4</v>
@@ -1054,7 +1047,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1071,7 +1064,7 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G21">
         <v>4</v>
@@ -1080,7 +1073,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1097,7 +1090,7 @@
         <v>8</v>
       </c>
       <c r="F22" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G22">
         <v>4</v>
@@ -1106,9 +1099,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>24679</v>
@@ -1132,7 +1125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P26" s="1"/>
     </row>
   </sheetData>

</xml_diff>